<commit_message>
broke up code into steps
</commit_message>
<xml_diff>
--- a/metadata/rlc_metadata_06202024.xlsx
+++ b/metadata/rlc_metadata_06202024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\github\anemone-leachate-heat\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minerva\Documents\GitHub\anemone-leachate-heat\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81932B9-96FB-4C90-9A6C-544CCECC3FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC718FE0-6796-468B-B433-108971816A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13305" yWindow="60" windowWidth="24945" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="76">
   <si>
     <t>No.</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>A. elegantissima x B. muscatinei</t>
+  </si>
+  <si>
+    <t>H4C</t>
   </si>
 </sst>
 </file>
@@ -568,18 +571,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14</v>
       </c>
@@ -634,7 +637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>27</v>
       </c>
@@ -660,7 +663,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>53</v>
       </c>
@@ -686,7 +689,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>67</v>
       </c>
@@ -712,7 +715,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>79</v>
       </c>
@@ -738,7 +741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>92</v>
       </c>
@@ -764,7 +767,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>105</v>
       </c>
@@ -790,7 +793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>118</v>
       </c>
@@ -816,7 +819,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>131</v>
       </c>
@@ -842,7 +845,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>144</v>
       </c>
@@ -868,7 +871,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>157</v>
       </c>
@@ -894,7 +897,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>171</v>
       </c>
@@ -920,7 +923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>184</v>
       </c>
@@ -946,7 +949,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>197</v>
       </c>
@@ -975,7 +978,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>210</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>223</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>236</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>249</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>262</v>
       </c>
@@ -1105,50 +1108,50 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>275</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>288</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22">
         <v>6</v>
-      </c>
-      <c r="G21" t="s">
-        <v>72</v>
-      </c>
-      <c r="I21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>301</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E22" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22">
-        <v>4</v>
       </c>
       <c r="G22" t="s">
         <v>72</v>
@@ -1157,12 +1160,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1177,56 +1180,56 @@
         <v>4</v>
       </c>
       <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>314</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
         <v>70</v>
       </c>
-      <c r="I23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24">
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>327</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25">
         <v>3</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-      <c r="I24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>340</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
       </c>
       <c r="G25" t="s">
         <v>72</v>
@@ -1235,157 +1238,157 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>340</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>353</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>2</v>
       </c>
-      <c r="D26" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="D27" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
         <v>70</v>
       </c>
-      <c r="I26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27">
+      <c r="I27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>366</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>34</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28">
         <v>7</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>72</v>
       </c>
-      <c r="I27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28">
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>379</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29">
         <v>8</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>71</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>22</v>
       </c>
-      <c r="I28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29">
+      <c r="I29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>392</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30">
         <v>4</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>70</v>
       </c>
-      <c r="I29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30">
+      <c r="I30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>405</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31">
         <v>10</v>
-      </c>
-      <c r="G30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>418</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E31" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31">
-        <v>8</v>
       </c>
       <c r="G31" t="s">
         <v>72</v>
@@ -1394,15 +1397,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="1">
         <v>45463</v>
@@ -1411,7 +1414,7 @@
         <v>68</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G32" t="s">
         <v>72</v>
@@ -1420,50 +1423,50 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>431</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>444</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34">
         <v>2</v>
-      </c>
-      <c r="G33" t="s">
-        <v>71</v>
-      </c>
-      <c r="I33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>457</v>
-      </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
       </c>
       <c r="G34" t="s">
         <v>71</v>
@@ -1472,180 +1475,180 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>457</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>470</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E35" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36">
         <v>8</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>70</v>
       </c>
-      <c r="I35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36">
+      <c r="I36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>483</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E36" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E37" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37">
         <v>7</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>72</v>
       </c>
-      <c r="I36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37">
+      <c r="I37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>496</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>71</v>
       </c>
-      <c r="I37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38">
+      <c r="I38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>522</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>45</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39">
         <v>6</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>70</v>
       </c>
-      <c r="I38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A39">
+      <c r="I39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>534</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F39">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40">
         <v>8</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>72</v>
       </c>
-      <c r="I39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40">
+      <c r="I40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>548</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>47</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E40" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41">
         <v>5</v>
-      </c>
-      <c r="G40" t="s">
-        <v>71</v>
-      </c>
-      <c r="I40" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>561</v>
-      </c>
-      <c r="B41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E41" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41">
-        <v>9</v>
       </c>
       <c r="G41" t="s">
         <v>71</v>
@@ -1654,50 +1657,50 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>561</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E42" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42" t="s">
+        <v>71</v>
+      </c>
+      <c r="I42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>574</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E42" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43">
         <v>2</v>
-      </c>
-      <c r="G42" t="s">
-        <v>70</v>
-      </c>
-      <c r="I42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>587</v>
-      </c>
-      <c r="B43" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43">
-        <v>10</v>
       </c>
       <c r="G43" t="s">
         <v>70</v>
@@ -1706,119 +1709,119 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>587</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>70</v>
+      </c>
+      <c r="I44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>600</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E44" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45">
         <v>9</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>71</v>
       </c>
-      <c r="I44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45">
+      <c r="I45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>613</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>52</v>
       </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E45" t="s">
-        <v>68</v>
-      </c>
-      <c r="F45">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46">
         <v>2</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>72</v>
       </c>
-      <c r="I45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46">
+      <c r="I46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>626</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>53</v>
       </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E46" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E47" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
         <v>70</v>
       </c>
-      <c r="I46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47">
+      <c r="I47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>639</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>54</v>
       </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F47">
-        <v>7</v>
-      </c>
-      <c r="G47" t="s">
-        <v>71</v>
-      </c>
-      <c r="I47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>652</v>
-      </c>
-      <c r="B48" t="s">
-        <v>55</v>
-      </c>
       <c r="C48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1">
         <v>45463</v>
@@ -1830,82 +1833,82 @@
         <v>7</v>
       </c>
       <c r="G48" t="s">
+        <v>71</v>
+      </c>
+      <c r="I48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>652</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E49" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
         <v>70</v>
       </c>
-      <c r="I48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A49">
+      <c r="I49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>665</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E49" t="s">
-        <v>69</v>
-      </c>
-      <c r="F49">
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E50" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50">
         <v>2</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>71</v>
       </c>
-      <c r="I49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A50">
+      <c r="I50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>677</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E50" t="s">
-        <v>69</v>
-      </c>
-      <c r="F50">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E51" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51">
         <v>3</v>
-      </c>
-      <c r="G50" t="s">
-        <v>72</v>
-      </c>
-      <c r="I50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>691</v>
-      </c>
-      <c r="B51" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E51" t="s">
-        <v>69</v>
-      </c>
-      <c r="F51">
-        <v>2</v>
       </c>
       <c r="G51" t="s">
         <v>72</v>
@@ -1914,76 +1917,76 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>691</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E52" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>72</v>
+      </c>
+      <c r="I52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>704</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>59</v>
       </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E52" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52">
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53">
         <v>6</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>71</v>
       </c>
-      <c r="I52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53">
+      <c r="I53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>717</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E53" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E54" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54">
         <v>5</v>
-      </c>
-      <c r="G53" t="s">
-        <v>70</v>
-      </c>
-      <c r="I53" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>729</v>
-      </c>
-      <c r="B54" t="s">
-        <v>61</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E54" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54">
-        <v>10</v>
       </c>
       <c r="G54" t="s">
         <v>70</v>
@@ -1992,142 +1995,142 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
+        <v>729</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E55" t="s">
+        <v>69</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+      <c r="G55" t="s">
+        <v>70</v>
+      </c>
+      <c r="I55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>743</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E55" t="s">
-        <v>68</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E56" t="s">
+        <v>68</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
         <v>72</v>
       </c>
-      <c r="I55" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A56">
+      <c r="I56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>756</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>63</v>
       </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E56" t="s">
-        <v>68</v>
-      </c>
-      <c r="F56">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E57" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57">
         <v>9</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G57" t="s">
         <v>70</v>
       </c>
-      <c r="I56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57">
+      <c r="I57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>769</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E57" t="s">
-        <v>68</v>
-      </c>
-      <c r="F57">
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E58" t="s">
+        <v>68</v>
+      </c>
+      <c r="F58">
         <v>5</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G58" t="s">
         <v>71</v>
       </c>
-      <c r="I57" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58">
+      <c r="I58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>782</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>65</v>
       </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E58" t="s">
-        <v>68</v>
-      </c>
-      <c r="F58">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E59" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59">
         <v>2</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>70</v>
       </c>
-      <c r="I58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59">
+      <c r="I59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>795</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>66</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" s="1">
-        <v>45463</v>
-      </c>
-      <c r="E59" t="s">
-        <v>68</v>
-      </c>
-      <c r="F59">
-        <v>10</v>
-      </c>
-      <c r="G59" t="s">
-        <v>71</v>
-      </c>
-      <c r="I59" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60">
-        <v>808</v>
-      </c>
-      <c r="B60" t="s">
-        <v>67</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2142,9 +2145,35 @@
         <v>10</v>
       </c>
       <c r="G60" t="s">
+        <v>71</v>
+      </c>
+      <c r="I60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>808</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <v>45463</v>
+      </c>
+      <c r="E61" t="s">
+        <v>68</v>
+      </c>
+      <c r="F61">
+        <v>10</v>
+      </c>
+      <c r="G61" t="s">
         <v>72</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I61" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>